<commit_message>
Corrección información de diccionarios
</commit_message>
<xml_diff>
--- a/6_Documentation/Dictionaries/diccionario _yelp.xlsx
+++ b/6_Documentation/Dictionaries/diccionario _yelp.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Henry\02. Course\3. Final Proyect\Commerce-Data-Analysis-and-Recommendations\Commerce-Data-Analysis-and-Recommendations\6_Documentation\Dictionaries\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1088B8-36AB-47DD-BC9B-8734E750E35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="business" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="rewievs" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="users" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="checkin" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="tips" sheetId="5" r:id="rId8"/>
+    <sheet name="business" sheetId="1" r:id="rId1"/>
+    <sheet name="rewievs" sheetId="2" r:id="rId2"/>
+    <sheet name="users" sheetId="3" r:id="rId3"/>
+    <sheet name="checkin" sheetId="4" r:id="rId4"/>
+    <sheet name="tips" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="105">
   <si>
     <t>Columna</t>
   </si>
@@ -336,38 +345,40 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="&quot;Quattrocento Sans&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -378,7 +389,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -388,7 +399,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFAEABAB"/>
@@ -402,8 +419,10 @@
       <bottom style="thin">
         <color rgb="FFAEABAB"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FFAEABAB"/>
       </right>
@@ -413,63 +432,43 @@
       <bottom style="thin">
         <color rgb="FFAEABAB"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -659,23 +658,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="80.25"/>
+    <col min="3" max="3" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -703,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -714,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -725,7 +729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -736,7 +740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -747,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -758,7 +762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -769,7 +773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -780,7 +784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -791,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -802,7 +806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -813,7 +817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -824,7 +828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -835,7 +839,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -847,24 +851,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="49.63"/>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -892,7 +899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>41</v>
       </c>
@@ -903,7 +910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -914,7 +921,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -925,7 +932,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -936,7 +943,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
@@ -947,7 +954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -958,7 +965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>51</v>
       </c>
@@ -969,7 +976,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -980,41 +987,44 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.88"/>
-    <col customWidth="1" min="3" max="3" width="57.25"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -1042,7 +1052,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1064,7 +1074,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>59</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -1097,7 +1107,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
@@ -1119,7 +1129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>68</v>
       </c>
@@ -1130,7 +1140,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1152,7 +1162,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>74</v>
       </c>
@@ -1163,7 +1173,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>76</v>
       </c>
@@ -1174,7 +1184,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>78</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>80</v>
       </c>
@@ -1196,7 +1206,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>82</v>
       </c>
@@ -1207,7 +1217,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>84</v>
       </c>
@@ -1218,7 +1228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>86</v>
       </c>
@@ -1229,7 +1239,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>88</v>
       </c>
@@ -1240,7 +1250,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>90</v>
       </c>
@@ -1251,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>92</v>
       </c>
@@ -1262,7 +1272,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>94</v>
       </c>
@@ -1274,24 +1284,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="51.63"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1319,7 +1332,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -1330,59 +1343,62 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="5"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.0"/>
-    <col customWidth="1" min="3" max="3" width="43.5"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1396,79 +1412,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="C5" s="3" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="5"/>
+      <c r="C7" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="5"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="5"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="5"/>
     </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="5"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>